<commit_message>
updated the contacts.xlsx by removing my personal data
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Projects\whatsapp_fixed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E589A8D-AC42-47CF-91B9-35B44B0896F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA43519-394D-49A9-B286-C80D7BCE8469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2160" yWindow="2160" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>phone</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>Greetings! This is a test.</t>
+  </si>
+  <si>
+    <t>phone no with country code</t>
+  </si>
+  <si>
+    <t>91xxxxxxxxx</t>
   </si>
 </sst>
 </file>
@@ -405,7 +411,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,24 +429,24 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>917068359697</v>
+      <c r="A2" t="s">
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>917068359697</v>
+      <c r="A3" t="s">
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>917068359697</v>
+      <c r="A4" t="s">
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>

</xml_diff>